<commit_message>
Fixed bug when first character equals '\='
</commit_message>
<xml_diff>
--- a/password.xlsx
+++ b/password.xlsx
@@ -12,13 +12,29 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Courier New"/>
+    </font>
+    <font>
+      <name val="Courier"/>
+      <color rgb="00BB56BB"/>
+    </font>
+    <font>
+      <name val="Courier"/>
+      <color rgb="00BB56BB"/>
+      <sz val="40"/>
+    </font>
+    <font>
+      <name val="Courier New"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -41,8 +57,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,172 +474,172 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>gmMR-Zy(;</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>S;@r/CY!=</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>s&gt;o$&lt;EN1V</t>
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>HieYg"vr+</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Nh*2eMf%C</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>O{NH(b#1`</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>3yju#{%O5</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>J*.mMRZc7</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>#dztG3'Ns</t>
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>s&lt;JE&amp;o"=v</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>n05lIBNTe</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>T@cA~|ujn</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>`Wz"2,Pp(</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>f@J?NuO_P</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>jHas_L2q[</t>
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>{D6RMm/v*</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>SJ[a^NoP:</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>PDr^,-Q)C</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>a~?&amp;@Jslb</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>]#a&gt;WAymB</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>RJH6XLGoB</t>
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>*D\?rVBOP</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>T&gt;`YsgrX5</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>^&lt;-(@{c7E</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SrqX=D_Te</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>)UXpHEmOD</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>oNfSLh}8I</t>
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>@mgK%(OWJ</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>9lugNo_^A</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>:_Yu@2Vhq</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>;3(W5"xZN</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>bC/,F&amp;)1s</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Lq^&gt;|Y7ay</t>
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>":P&gt;k_~sd</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>4y9}Q5J=w</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>ojR4&gt;cpVJ</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>#wD?8c,ti</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>dJ/{WXD`a</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Ozw=,&gt;F.e</t>
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>-]rt)}L+&gt;</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>}d%#"[!j6</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>LScvDFk4&lt;</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Xlx5[h+v@</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>$:rV;0Hc&lt;</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>\z:j)mTuW</t>
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>h{`7|SFk}</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>ng|oGS~`p</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>wA?:.-mvD</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>xQk+nvj-i</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>w|MLjx2v5</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>A98PHLCy{</t>
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>e/*!~z0}(</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>ZbKm~-X=c</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>nW~[]1N:!</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>#71lC6&amp;Ea</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>G|7#lDogT</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>/\.+*d,;b</t>
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>%`-_4S(Zf</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>Bve5&amp;9Qyr</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>HG@[8v}W5</t>
         </is>
       </c>
     </row>

</xml_diff>